<commit_message>
added summary stats to excel table
</commit_message>
<xml_diff>
--- a/writing/output_table.xlsx
+++ b/writing/output_table.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Duncan_Lab_2018\NHANES_WeightPerception\NHANES_wt\writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F383E-FCE1-40AA-A30A-B5DD76383A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="114_{46F66201-AA45-4D74-A00B-83FED43E67CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC6A852-912B-44E6-8A6B-1D90168F415F}"/>
   <bookViews>
-    <workbookView xWindow="11213" yWindow="458" windowWidth="10380" windowHeight="12892" activeTab="2" xr2:uid="{64D5762E-E7CA-4964-B70E-AD8288C837C3}"/>
+    <workbookView xWindow="1747" yWindow="1357" windowWidth="18211" windowHeight="12893" activeTab="3" xr2:uid="{64D5762E-E7CA-4964-B70E-AD8288C837C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression_All" sheetId="1" r:id="rId1"/>
     <sheet name="Reg_Male" sheetId="3" r:id="rId2"/>
     <sheet name="Reg_Female" sheetId="4" r:id="rId3"/>
-    <sheet name="Correlations" sheetId="2" r:id="rId4"/>
+    <sheet name="SummaryTable" sheetId="5" r:id="rId4"/>
+    <sheet name="Correlations" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="379">
   <si>
     <t>Like to Weigh Less</t>
   </si>
@@ -1134,6 +1135,45 @@
   </si>
   <si>
     <t>1.11 (1.05 - 1.17)</t>
+  </si>
+  <si>
+    <t>Not sig different</t>
+  </si>
+  <si>
+    <t>Sig different</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Smoking (Former)</t>
+  </si>
+  <si>
+    <t>Smoking (Current)</t>
+  </si>
+  <si>
+    <t>Cannabis Use (Ordinal)</t>
+  </si>
+  <si>
+    <t>Cannabis Use (Ever)</t>
+  </si>
+  <si>
+    <t>Like to Weigh More</t>
+  </si>
+  <si>
+    <t>Consider Weight Too Big</t>
+  </si>
+  <si>
+    <t>Lost Weight Intentionally</t>
+  </si>
+  <si>
+    <t>Lost Weight Unintentionally</t>
+  </si>
+  <si>
+    <t>Tried to Lose Weight</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1210,6 +1250,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1223,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1302,7 +1354,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1643,16 +1713,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
@@ -1891,16 +1961,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="22"/>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="F15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="20"/>
@@ -2143,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2A9C5E-8065-457A-B0D1-F5EA1BBFC0AA}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="G20" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
@@ -2161,11 +2231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="F1" s="30" t="s">
+        <v>366</v>
+      </c>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -2177,6 +2250,9 @@
       </c>
       <c r="D2" s="18" t="s">
         <v>26</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>367</v>
       </c>
       <c r="J2" s="17"/>
     </row>
@@ -2227,7 +2303,7 @@
       <c r="C6" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="24" t="s">
         <v>234</v>
       </c>
       <c r="I6" s="11"/>
@@ -2243,7 +2319,7 @@
       <c r="C7" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="24" t="s">
         <v>237</v>
       </c>
       <c r="F7" s="16"/>
@@ -2334,16 +2410,16 @@
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="F15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="18" t="s">
@@ -2663,7 +2739,7 @@
       <c r="G34" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="36" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2686,7 +2762,7 @@
       <c r="G35" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="36" t="s">
         <v>361</v>
       </c>
     </row>
@@ -2802,8 +2878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F15C75A-2FAA-4192-95E2-C7899D95EA36}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="D22" zoomScale="81" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
@@ -2820,11 +2896,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -2995,16 +3071,16 @@
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="F15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="17" t="s">
@@ -3135,7 +3211,7 @@
       <c r="C23" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="31" t="s">
         <v>169</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -3485,6 +3561,461 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918B3E14-A501-451B-9F97-9B8718EA1473}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="37">
+        <v>3.51</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="37">
+        <v>1.41</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="37">
+        <v>2.11</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1.77</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B7" s="37">
+        <v>3.04</v>
+      </c>
+      <c r="C7" s="37">
+        <v>1.29</v>
+      </c>
+      <c r="D7" s="37">
+        <v>1.75</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>375</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="37">
+        <v>1.34</v>
+      </c>
+      <c r="F9" s="37">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="37">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="37">
+        <v>1.24</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="37">
+        <v>1.54</v>
+      </c>
+      <c r="D18" s="37">
+        <v>0.79</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="37">
+        <v>1.41</v>
+      </c>
+      <c r="D19" s="37">
+        <v>1.33</v>
+      </c>
+      <c r="E19" s="37">
+        <v>1.38</v>
+      </c>
+      <c r="F19" s="37">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B21" s="37">
+        <v>1.43</v>
+      </c>
+      <c r="C21" s="37">
+        <v>1.32</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="37">
+        <v>2.25</v>
+      </c>
+      <c r="C22" s="37">
+        <v>1.51</v>
+      </c>
+      <c r="D22" s="37">
+        <v>1.61</v>
+      </c>
+      <c r="E22" s="37">
+        <v>1.63</v>
+      </c>
+      <c r="F22" s="37">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>375</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="37">
+        <v>1.28</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>376</v>
+      </c>
+      <c r="B25" s="37">
+        <v>2.38</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="37">
+        <v>1.45</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>377</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="37">
+        <v>0.61</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:F27">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53F5B2A-72BC-48DB-B075-46F5B78F74C9}">
   <dimension ref="A1:D17"/>
   <sheetViews>

</xml_diff>

<commit_message>
added looking at patterns of what people do to lose weight
</commit_message>
<xml_diff>
--- a/writing/output_table.xlsx
+++ b/writing/output_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Duncan_Lab_2018\NHANES_WeightPerception\NHANES_wt\writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="114_{46F66201-AA45-4D74-A00B-83FED43E67CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC6A852-912B-44E6-8A6B-1D90168F415F}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="114_{46F66201-AA45-4D74-A00B-83FED43E67CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B990B8A-432F-48A7-9020-19AAD8BD30F5}"/>
   <bookViews>
-    <workbookView xWindow="1747" yWindow="1357" windowWidth="18211" windowHeight="12893" activeTab="3" xr2:uid="{64D5762E-E7CA-4964-B70E-AD8288C837C3}"/>
+    <workbookView xWindow="2655" yWindow="540" windowWidth="18210" windowHeight="12893" activeTab="3" xr2:uid="{64D5762E-E7CA-4964-B70E-AD8288C837C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression_All" sheetId="1" r:id="rId1"/>
@@ -1275,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1354,15 +1354,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1373,6 +1364,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1713,16 +1716,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="F1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
@@ -1961,16 +1964,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="22"/>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="F15" s="33" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="F15" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="20"/>
@@ -2231,11 +2234,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="F1" s="30" t="s">
         <v>366</v>
       </c>
@@ -2251,7 +2254,7 @@
       <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="32" t="s">
         <v>367</v>
       </c>
       <c r="J2" s="17"/>
@@ -2410,16 +2413,16 @@
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="F15" s="33" t="s">
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="F15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="18" t="s">
@@ -2739,7 +2742,7 @@
       <c r="G34" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="H34" s="36" t="s">
+      <c r="H34" s="33" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2762,7 +2765,7 @@
       <c r="G35" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="H35" s="36" t="s">
+      <c r="H35" s="33" t="s">
         <v>361</v>
       </c>
     </row>
@@ -2896,11 +2899,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -3071,16 +3074,16 @@
       <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="F15" s="33" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="F15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="17" t="s">
@@ -3565,7 +3568,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3582,26 +3585,26 @@
       <c r="A1" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="34" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3609,19 +3612,19 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="34">
         <v>3.51</v>
       </c>
-      <c r="C3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="37">
+      <c r="C3" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="34">
         <v>1.41</v>
       </c>
-      <c r="E3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3629,46 +3632,46 @@
       <c r="A4" t="s">
         <v>373</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="37">
+      <c r="B4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="34">
         <v>2.11</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="37">
+      <c r="D4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="34">
         <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="37">
+      <c r="B6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="34">
         <v>1.77</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="38" t="s">
+      <c r="D6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3676,46 +3679,46 @@
       <c r="A7" t="s">
         <v>374</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="34">
         <v>3.04</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="34">
         <v>1.29</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="34">
         <v>1.75</v>
       </c>
-      <c r="E7" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="38" t="s">
+      <c r="E7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>375</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="37">
+      <c r="B9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="34">
         <v>1.34</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="34">
         <v>1.06</v>
       </c>
     </row>
@@ -3723,19 +3726,19 @@
       <c r="A10" t="s">
         <v>376</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="34">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="37">
+      <c r="C10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="39">
         <v>1.5</v>
       </c>
-      <c r="E10" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="38" t="s">
+      <c r="E10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3743,19 +3746,19 @@
       <c r="A11" t="s">
         <v>377</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="37">
+      <c r="B11" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="34">
         <v>1.24</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="34">
         <v>0.8</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="38" t="s">
+      <c r="E11" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3763,67 +3766,67 @@
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="34">
         <v>0.54</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="38" t="s">
+      <c r="C12" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="37"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>378</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="34" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3831,19 +3834,19 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="37">
+      <c r="B18" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="34">
         <v>1.54</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="34">
         <v>0.79</v>
       </c>
-      <c r="E18" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="38" t="s">
+      <c r="E18" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3851,46 +3854,46 @@
       <c r="A19" t="s">
         <v>373</v>
       </c>
-      <c r="B19" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="37">
+      <c r="B19" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="34">
         <v>1.41</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="34">
         <v>1.33</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="34">
         <v>1.38</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="34">
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>374</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="34">
         <v>1.43</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="34">
         <v>1.32</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="37">
+      <c r="D21" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="34">
         <v>1.06</v>
       </c>
     </row>
@@ -3898,46 +3901,46 @@
       <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="37">
+      <c r="B22" s="34">
         <v>2.25</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="34">
         <v>1.51</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="34">
         <v>1.61</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="34">
         <v>1.63</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="34">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>375</v>
       </c>
-      <c r="B24" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="37">
+      <c r="B24" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="34">
         <v>1.28</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="38" t="s">
+      <c r="D24" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3945,19 +3948,19 @@
       <c r="A25" t="s">
         <v>376</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="34">
         <v>2.38</v>
       </c>
-      <c r="C25" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="37">
+      <c r="C25" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="34">
         <v>1.45</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3965,19 +3968,19 @@
       <c r="A26" t="s">
         <v>377</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="37">
+      <c r="B26" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="39">
         <v>0.6</v>
       </c>
-      <c r="E26" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="38" t="s">
+      <c r="E26" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="35" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3985,33 +3988,49 @@
       <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="37">
+      <c r="B27" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="34">
         <v>0.61</v>
       </c>
-      <c r="E27" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="38" t="s">
+      <c r="E27" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="35" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F27">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="3Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{C085498E-8CFD-45D3-899B-EECC4660180C}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="4Arrows" iconId="2"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B1:F27</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>